<commit_message>
[improvements] - [`nexial.lastOutputLink`]: update this System variable for files being generated locally in a "output-to-cloud" execution (which subsequently transferred such file to the cloud). - generate dedicated error log file for error or failure that occurred during execution.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/start-01.data.xlsx
+++ b/artifact/data/start-01.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A586B33-2608-AD47-81F3-8B72E7F5F480}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A64B09-456E-4249-B816-E619C5C7066E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="6840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="6840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -53,30 +53,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
   <si>
     <t>nexial.pollWaitMs</t>
-  </si>
-  <si>
-    <t>nexial.failFast</t>
-  </si>
-  <si>
-    <t>nexial.textDelim</t>
-  </si>
-  <si>
-    <t>nexial.verbose</t>
   </si>
   <si>
     <t>nexial.openResult</t>
@@ -918,9 +903,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA20"/>
+  <dimension ref="A1:AAA17"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -934,7 +919,7 @@
   <sheetData>
     <row r="1" spans="1:703" ht="24" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -944,30 +929,30 @@
     </row>
     <row r="2" spans="1:703" ht="24" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703" ht="24" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703" ht="24" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
@@ -977,54 +962,27 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703" ht="24" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703" ht="24" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="HA7" s="4"/>
-      <c r="AAA7" s="5"/>
-    </row>
-    <row r="8" spans="1:703" ht="24" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="HA8" s="4"/>
-      <c r="AAA8" s="5"/>
-    </row>
-    <row r="9" spans="1:703" ht="24" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-    <row r="10" spans="1:703" ht="24" customHeight="1">
-      <c r="B10" s="7"/>
-    </row>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:703" ht="24" customHeight="1"/>
+    <row r="9" spans="1:703" ht="24" customHeight="1"/>
+    <row r="10" spans="1:703" ht="24" customHeight="1"/>
     <row r="11" spans="1:703" ht="24" customHeight="1"/>
     <row r="12" spans="1:703" ht="24" customHeight="1"/>
     <row r="13" spans="1:703" ht="24" customHeight="1"/>
@@ -1032,9 +990,6 @@
     <row r="15" spans="1:703" ht="24" customHeight="1"/>
     <row r="16" spans="1:703" ht="24" customHeight="1"/>
     <row r="17" ht="24" customHeight="1"/>
-    <row r="18" ht="24" customHeight="1"/>
-    <row r="19" ht="24" customHeight="1"/>
-    <row r="20" ht="24" customHeight="1"/>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
@@ -1081,20 +1036,20 @@
   <sheetData>
     <row r="1" spans="1:703" ht="24" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703" ht="24" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
@@ -1204,27 +1159,27 @@
   <sheetData>
     <row r="1" spans="1:703" ht="24" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703" ht="24" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="HA2" s="4"/>
       <c r="AAA2" s="5"/>
     </row>
     <row r="3" spans="1:703" ht="24" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
@@ -1300,9 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63120A5B-2C90-0346-AF50-5EFE2AC7C134}">
   <dimension ref="A1:AAA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -1411,20 +1364,20 @@
   <sheetData>
     <row r="1" spans="1:703" ht="24" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703" ht="24" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="HA2" s="4"/>
       <c r="AAA2" s="5"/>

</xml_diff>